<commit_message>
push algoritmo fixes and algoritmo 2
</commit_message>
<xml_diff>
--- a/BipartiteKnapsackProblem/inputs/Algoritmo.xlsx
+++ b/BipartiteKnapsackProblem/inputs/Algoritmo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Adrian\Github\BipartiteKnapsackProblem\BipartiteKnapsackProblem\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0ACA82-204E-49BF-9630-F66AD2769A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60F7CA4-7EE4-4B05-B056-B92F8AB258DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="615" yWindow="735" windowWidth="16590" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avance de camion" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Optimisation camion salumi'!$A$1:$G$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Optimisation salumi'!$A$1:$G$29</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0" concurrentManualCount="1"/>
+  <calcPr calcId="191029" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5730,7 +5730,7 @@
   <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H29"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>